<commit_message>
CitiesPrep with apt. prices (done)
</commit_message>
<xml_diff>
--- a/migforecasting/datasets/AvgAptPrices.xlsx
+++ b/migforecasting/datasets/AvgAptPrices.xlsx
@@ -3045,9 +3045,6 @@
     <t>Тюмень</t>
   </si>
   <si>
-    <t xml:space="preserve">            Ханты-Мансийск</t>
-  </si>
-  <si>
     <t>Салехард</t>
   </si>
   <si>
@@ -3115,18 +3112,29 @@
   </si>
   <si>
     <t>Биробиджан</t>
+  </si>
+  <si>
+    <t>Ханты-Мансийск</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -3170,16 +3178,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3488,8 +3499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M99"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S8" sqref="S8"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="T47" sqref="T47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5929,8 +5940,8 @@
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A60" s="4" t="s">
-        <v>1008</v>
+      <c r="A60" s="5" t="s">
+        <v>1031</v>
       </c>
       <c r="B60" s="4" t="s">
         <v>682</v>
@@ -5971,7 +5982,7 @@
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="B61" s="4" t="s">
         <v>694</v>
@@ -6012,7 +6023,7 @@
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="B62" s="4" t="s">
         <v>706</v>
@@ -6053,7 +6064,7 @@
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="B63" s="4" t="s">
         <v>718</v>
@@ -6089,12 +6100,12 @@
         <v>728</v>
       </c>
       <c r="M63" s="4" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="B64" s="4" t="s">
         <v>729</v>
@@ -6130,12 +6141,12 @@
         <v>728</v>
       </c>
       <c r="M64" s="4" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="B65" s="4" t="s">
         <v>737</v>
@@ -6176,7 +6187,7 @@
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="B66" s="4" t="s">
         <v>749</v>
@@ -6217,7 +6228,7 @@
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="B67" s="4" t="s">
         <v>761</v>
@@ -6258,7 +6269,7 @@
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="B68" s="4" t="s">
         <v>773</v>
@@ -6299,7 +6310,7 @@
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="B69" s="4" t="s">
         <v>785</v>
@@ -6340,7 +6351,7 @@
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="B70" s="4" t="s">
         <v>797</v>
@@ -6381,7 +6392,7 @@
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="B71" s="4" t="s">
         <v>809</v>
@@ -6422,7 +6433,7 @@
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="B72" s="4" t="s">
         <v>821</v>
@@ -6463,7 +6474,7 @@
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="B73" s="4" t="s">
         <v>833</v>
@@ -6504,7 +6515,7 @@
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="B74" s="4" t="s">
         <v>845</v>
@@ -6545,7 +6556,7 @@
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="B75" s="4" t="s">
         <v>857</v>
@@ -6586,7 +6597,7 @@
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="B76" s="4" t="s">
         <v>869</v>
@@ -6627,7 +6638,7 @@
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="B77" s="4" t="s">
         <v>881</v>
@@ -6668,7 +6679,7 @@
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="B78" s="4" t="s">
         <v>893</v>
@@ -6709,7 +6720,7 @@
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="B79" s="4" t="s">
         <v>905</v>
@@ -6750,7 +6761,7 @@
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="B80" s="4" t="s">
         <v>917</v>
@@ -6791,7 +6802,7 @@
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="B81" s="4" t="s">
         <v>926</v>
@@ -6832,7 +6843,7 @@
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="B82" s="4" t="s">
         <v>938</v>

</xml_diff>